<commit_message>
minor changes to admin filing system
</commit_message>
<xml_diff>
--- a/Admin Files/Who Doin Wat.xlsx
+++ b/Admin Files/Who Doin Wat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685B5F68-F6AD-48EE-8D75-F9060BD02C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9B31F7-99E2-46EE-9F20-A0AFF13080D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7AA417BD-2748-4CDC-B273-67AFD46A09ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7AA417BD-2748-4CDC-B273-67AFD46A09ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="2" r:id="rId1"/>
@@ -652,24 +652,24 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" style="11" customWidth="1"/>
-    <col min="7" max="11" width="17.88671875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="11" customWidth="1"/>
+    <col min="7" max="11" width="17.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="16" t="s">
         <v>0</v>
@@ -686,7 +686,7 @@
       <c r="L1" s="16"/>
       <c r="M1" s="16"/>
     </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -727,7 +727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>14</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>16</v>
       </c>
@@ -805,7 +805,7 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>17</v>
       </c>
@@ -831,7 +831,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>18</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:18" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
@@ -883,7 +883,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
@@ -909,15 +909,15 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -935,15 +935,15 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -961,7 +961,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -981,7 +981,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -996,7 +996,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1011,7 +1011,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1026,7 +1026,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1041,7 +1041,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1056,7 +1056,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>

</xml_diff>